<commit_message>
test video, mute=1 for autoplay
</commit_message>
<xml_diff>
--- a/_Notes/events.xlsx
+++ b/_Notes/events.xlsx
@@ -738,26 +738,26 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L7" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.89795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="257.025510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="117.352040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5969387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="91.9744897959184"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="176.030612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="236.326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="33.2959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="328.301020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="149.928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.6989795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="117.352040816327"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="224.80612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="302.020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="42.4795918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,7 +1015,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="430.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="198.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>59</v>
       </c>

</xml_diff>